<commit_message>
Changes to IMG and video API
</commit_message>
<xml_diff>
--- a/movies.xlsx
+++ b/movies.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\vistr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63953C8-AC86-4FD9-AF95-D39F714EEAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="VideoData" r:id="rId3" sheetId="1"/>
+    <sheet name="VideoData" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -44,20 +52,19 @@
     <t>TA</t>
   </si>
   <si>
-    <t>J:\originserverdb\images\GURU_2007.jpg</t>
-  </si>
-  <si>
-    <t>J:\originserverdb\VID2.mp4</t>
+    <t>GURU_2007.jpg</t>
+  </si>
+  <si>
+    <t>VID2.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -69,7 +76,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -87,18 +94,328 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -118,7 +435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -139,6 +456,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes related to origin server
</commit_message>
<xml_diff>
--- a/movies.xlsx
+++ b/movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\vistr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63953C8-AC86-4FD9-AF95-D39F714EEAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15384BFD-21F1-4655-88A0-8C8B97EEC765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>TITLE</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Based on the life of Dhirubai Ambani</t>
   </si>
   <si>
-    <t>70</t>
-  </si>
-  <si>
     <t>TA</t>
   </si>
   <si>
@@ -56,19 +53,72 @@
   </si>
   <si>
     <t>VID2.mp4</t>
+  </si>
+  <si>
+    <t>Avatar: The Last Airbender</t>
+  </si>
+  <si>
+    <t>"The Boy in the Iceberg": Aang emerges from a century-long sleep and joins Katara and Sokka on a new adventure.</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>Avatar_S01E01.mp4</t>
+  </si>
+  <si>
+    <t>Avatar_S01E02.mp4</t>
+  </si>
+  <si>
+    <t>Avatar_S01E03.mp4</t>
+  </si>
+  <si>
+    <t>"The Avatar Returns": Aang faces the Fire Nation's pursuit while trying to protect his newfound friends.</t>
+  </si>
+  <si>
+    <t>"The Southern Air Temple": Aang grapples with the loss of his people while discovering the remnants of his past.</t>
+  </si>
+  <si>
+    <t>ATLA_S1E1.jpg</t>
+  </si>
+  <si>
+    <t>ATLA_S1E2.jpg</t>
+  </si>
+  <si>
+    <t>ATLA_S1E3.jpg</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,8 +141,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,55 +464,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>